<commit_message>
Update Ley Marco de Cambio Climático 21455_ 2022.xlsx
</commit_message>
<xml_diff>
--- a/Ley CC/Ley Marco de Cambio Climático 21455_ 2022.xlsx
+++ b/Ley CC/Ley Marco de Cambio Climático 21455_ 2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA INTELLIGENCE Dropbox\DI Monitoreo II\Ley CC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF64F19-CAD7-47D5-9DB7-BD964FF2D0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA345880-55C3-49CA-B59C-019E539C4D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{4A133405-1FDD-467B-BBEB-17B0081A62A5}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId3"/>
+    <pivotCache cacheId="9" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2615" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2641" uniqueCount="591">
   <si>
     <t>DISPOSICIONES GENERALES</t>
   </si>
@@ -2120,6 +2120,9 @@
   </si>
   <si>
     <t>ARTÍCULOS TRANSITORIOS</t>
+  </si>
+  <si>
+    <t>Artículos Transitorios</t>
   </si>
 </sst>
 </file>
@@ -7469,7 +7472,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D703CD75-7751-44AA-94B5-B3468022237D}" name="TablaDinámica1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D703CD75-7751-44AA-94B5-B3468022237D}" name="TablaDinámica1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:C24" firstHeaderRow="1" firstDataRow="1" firstDataCol="3"/>
   <pivotFields count="14">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -8596,9 +8599,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7468216D-F42E-480B-ACD7-43FBEBBB5A97}">
   <dimension ref="A12:N310"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="12" topLeftCell="A293" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F310" sqref="F310"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="12" topLeftCell="A310" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J318" sqref="J318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -20405,7 +20408,7 @@
         <v>No Contiene</v>
       </c>
     </row>
-    <row r="258" spans="1:14" ht="24" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:14" ht="36" x14ac:dyDescent="0.3">
       <c r="A258" s="2" t="s">
         <v>360</v>
       </c>
@@ -21658,7 +21661,9 @@
         <f>+LeyCC[[#This Row],[Artículo]]&amp;". "&amp;LeyCC[[#This Row],[Texto Artículo]]</f>
         <v>Artículo 47. Modificaciones en la ley N° 20.417. Modifícase el ARTÍCULO SEGUNDO de la ley N° 20.417, que crea la Superintendencia del Medio Ambiente y fija su ley orgánica, en el siguiente sentido:</v>
       </c>
-      <c r="J285" s="1"/>
+      <c r="J285" s="1" t="s">
+        <v>453</v>
+      </c>
       <c r="K285" s="6">
         <v>9</v>
       </c>
@@ -21704,7 +21709,9 @@
 Para estos efectos, la Superintendencia administrará un sistema de acreditación de personas naturales y jurídicas que realicen estas evaluaciones y verificaciones. El Reglamento determinará los requisitos, condiciones y procedimientos necesarios para su administración y funcionamiento, el que deberá, a lo menos, considerar la incompatibilidad absoluta entre el ejercicio de labores de evaluación y verificación y las de consultoría para la elaboración de proyectos de reducción o absorción de emisiones.
 Las infracciones a este literal se sancionarán de conformidad con lo dispuesto en el Título III de la presente ley, encontrándose la Superintendencia facultada, además, para revocar el certificado, rótulo o etiqueta como sanción.".</v>
       </c>
-      <c r="J286" s="1"/>
+      <c r="J286" s="1" t="s">
+        <v>453</v>
+      </c>
       <c r="K286" s="6">
         <v>9</v>
       </c>
@@ -21748,7 +21755,9 @@
         <v>Artículo 47 [2] Reemplázase el literal h) del artículo 35 por el siguiente:
 "h) El incumplimiento de las Normas de Emisión y de las Normas de Emisión de Gases de Efecto Invernadero.".</v>
       </c>
-      <c r="J287" s="1"/>
+      <c r="J287" s="1" t="s">
+        <v>453</v>
+      </c>
       <c r="K287" s="6">
         <v>9</v>
       </c>
@@ -21788,7 +21797,9 @@
         <f>+LeyCC[[#This Row],[Artículo]]&amp;". "&amp;LeyCC[[#This Row],[Texto Artículo]]</f>
         <v>Artículo 48. Modificaciones en la ley N° 20.600. Introdúcense las siguientes enmiendas en la ley N° 20.600, que Crea los Tribunales Ambientales:</v>
       </c>
-      <c r="J288" s="1"/>
+      <c r="J288" s="1" t="s">
+        <v>453</v>
+      </c>
       <c r="K288" s="6">
         <v>9</v>
       </c>
@@ -21833,7 +21844,9 @@
 "9) Conocer de las reclamaciones que se interpongan en contra de los decretos supremos que establezcan las normas de emisión de gases de efecto invernadero. Será competente el tribunal que en primer lugar se avoque a su consideración, excluyendo la competencia de los demás.
 10) Conocer de las reclamaciones que se interpongan en contra de las resoluciones que se pronuncien sobre la procedencia de un proyecto de reducción o absorción de emisiones de gases de efecto invernadero. Será competente para conocer de esta reclamación el Tribunal Ambiental del lugar en que se haya dictado la referida resolución.".</v>
       </c>
-      <c r="J289" s="1"/>
+      <c r="J289" s="1" t="s">
+        <v>453</v>
+      </c>
       <c r="K289" s="6">
         <v>9</v>
       </c>
@@ -21878,7 +21891,9 @@
 "8) En el caso del número 9), cualquier persona que considere que los decretos que tal numeral menciona no se ajustan a la ley.
 9) En el caso del número 10), las personas naturales o jurídicas directamente afectadas por la resolución del Ministerio del Medio Ambiente.".</v>
       </c>
-      <c r="J290" s="1"/>
+      <c r="J290" s="1" t="s">
+        <v>453</v>
+      </c>
       <c r="K290" s="6">
         <v>9</v>
       </c>
@@ -21921,7 +21936,9 @@
         <f>+LeyCC[[#This Row],[Artículo]]&amp;" ["&amp;LeyCC[[#This Row],[letra/número]]&amp;"] "&amp;LeyCC[[#This Row],[Texto Artículo]]</f>
         <v>Artículo 48 [3] Reemplázase, en el inciso tercero del artículo 26, la expresión "y 8)" por ", 8), 9) y 10)".</v>
       </c>
-      <c r="J291" s="1"/>
+      <c r="J291" s="1" t="s">
+        <v>453</v>
+      </c>
       <c r="K291" s="6">
         <v>9</v>
       </c>
@@ -21961,7 +21978,9 @@
         <f>+LeyCC[[#This Row],[Artículo]]&amp;". "&amp;LeyCC[[#This Row],[Texto Artículo]]</f>
         <v>Artículo 49. Modifícase el decreto con fuerza de ley N° 1, del Ministerio del Interior, de 2005, que fija el texto refundido, coordinado y sistematizado de la ley N° 19.175, orgánica constitucional sobre Gobierno y Administración Regional, de la manera que sigue:</v>
       </c>
-      <c r="J292" s="1"/>
+      <c r="J292" s="1" t="s">
+        <v>453</v>
+      </c>
       <c r="K292" s="6">
         <v>9</v>
       </c>
@@ -22005,7 +22024,9 @@
         <v>Artículo 49 [1] En el artículo 16, incorpórase la siguiente letra o), nueva:
 "o) Coparticipar con el Comité Regional para el cambio climático en la elaboración y aprobación de los instrumentos para la gestión del cambio climático a nivel regional.".</v>
       </c>
-      <c r="J293" s="1"/>
+      <c r="J293" s="1" t="s">
+        <v>453</v>
+      </c>
       <c r="K293" s="6">
         <v>9</v>
       </c>
@@ -22049,7 +22070,9 @@
         <v>Artículo 49 [2] En el artículo 17, sustitúyese el párrafo primero de la letra a) por el siguiente:
 "a) Elaborar y aprobar el plan regional de ordenamiento territorial en coherencia con la estrategia regional de desarrollo, la política nacional de ordenamiento territorial, la estrategia climática de largo plazo y el plan de acción regional de cambio climático, previo informe favorable de los ministros que conforman la Comisión Interministerial de Ciudad, Vivienda y Territorio, establecida en el párrafo quinto de este literal.".</v>
       </c>
-      <c r="J294" s="1"/>
+      <c r="J294" s="1" t="s">
+        <v>453</v>
+      </c>
       <c r="K294" s="6">
         <v>9</v>
       </c>
@@ -22093,7 +22116,9 @@
         <v>Artículo 49 [3] En el artículo 20, incorpórase la siguiente letra m), nueva:
 "m) Coparticipar con el Comité Regional para el cambio climático en la elaboración y aprobación de los instrumentos para la gestión del cambio climático a nivel regional.".</v>
       </c>
-      <c r="J295" s="1"/>
+      <c r="J295" s="1" t="s">
+        <v>453</v>
+      </c>
       <c r="K295" s="6">
         <v>9</v>
       </c>
@@ -22134,7 +22159,9 @@
         <v>Artículo 50. Reemplázase el inciso primero del artículo 10 de la ley N° 18.045, de Mercado de Valores, por el siguiente:
 "Artículo 10.- Las entidades inscritas en el Registro de Valores quedarán sujetas a esta ley y a sus normas complementarias y deberán proporcionar a la Comisión y al público en general, la información exigida por esta ley y por la Comisión, de conformidad a una norma de carácter general emitida por esta última. Dicha norma deberá exigir, a lo menos, información referida a los impactos ambientales y de cambio climático de las entidades inscritas, incluyendo la identificación, evaluación y gestión de los riesgos relacionados con esos factores, junto a las correspondientes métricas. La Comisión deberá especificar la forma, la publicidad y la periodicidad de la información a entregar por parte de las entidades inscritas, la que al menos será anual. En la elaboración de la citada normativa, la Comisión considerará estándares o recomendaciones nacionales o internacionales sobre la materia.".</v>
       </c>
-      <c r="J296" s="1"/>
+      <c r="J296" s="1" t="s">
+        <v>453</v>
+      </c>
       <c r="K296" s="6">
         <v>9</v>
       </c>
@@ -22174,7 +22201,9 @@
         <f>+LeyCC[[#This Row],[Artículo]]&amp;". "&amp;LeyCC[[#This Row],[Texto Artículo]]</f>
         <v>Artículo 51. Agréganse las siguientes oraciones finales nuevas en el inciso final del artículo 48 contenido en el artículo primero de la ley N° 20.712, sobre Administración de Fondos de Terceros y Carteras Individuales: "A su vez, las mencionadas políticas deberán incluir la información que la Comisión para el Mercado Financiero exija mediante norma de carácter general, la que deberá requerir, a lo menos, la forma en que se incorporan factores ambientales, en particular información referida a los impactos ambientales y al cambio climático, en su estrategia, gobierno corporativo, gestión de riesgos y decisiones de inversión y diversificación. Para estos efectos, la Comisión considerará estándares o recomendaciones nacionales o internacionales sobre la materia.".</v>
       </c>
-      <c r="J297" s="1"/>
+      <c r="J297" s="1" t="s">
+        <v>453</v>
+      </c>
       <c r="K297" s="6">
         <v>9</v>
       </c>
@@ -22214,7 +22243,9 @@
         <f>+LeyCC[[#This Row],[Artículo]]&amp;". "&amp;LeyCC[[#This Row],[Texto Artículo]]</f>
         <v>Artículo 52. Agréganse las siguientes oraciones finales en el inciso tercero del artículo 50 del decreto ley N° 3.500, que establece nuevo sistema de pensiones: "Adicionalmente, dicha norma deberá exigir, como materia mínima a incorporar en las respectivas políticas, la forma en que las administradoras incorporan factores ambientales, en particular información referida a los impactos ambientales y al cambio climático, en su estrategia, gobierno corporativo, gestión de riesgos y decisiones de inversión y diversificación. Para estos efectos, la Superintendencia considerará estándares o recomendaciones nacionales o internacionales sobre la materia.".</v>
       </c>
-      <c r="J298" s="1"/>
+      <c r="J298" s="1" t="s">
+        <v>453</v>
+      </c>
       <c r="K298" s="6">
         <v>9</v>
       </c>
@@ -22254,7 +22285,9 @@
         <f>+LeyCC[[#This Row],[Artículo]]&amp;". "&amp;LeyCC[[#This Row],[Texto Artículo]]</f>
         <v>Artículo 53. Modifícase la ley N° 20.530, que crea el Ministerio de Desarrollo Social y Familia, de la manera que sigue:</v>
       </c>
-      <c r="J299" s="1"/>
+      <c r="J299" s="1" t="s">
+        <v>453</v>
+      </c>
       <c r="K299" s="6">
         <v>9</v>
       </c>
@@ -22298,7 +22331,9 @@
         <v>Artículo 53 [1] Reemplázase el inciso sexto del artículo 1° por el siguiente: 
 "Corresponderá también a este Ministerio evaluar las iniciativas de inversión que solicitan financiamiento del Estado, para determinar su rentabilidad social, y velar por la eficacia y eficiencia del uso de los fondos públicos y la disminución de los efectos adversos del cambio climático, de manera que respondan a las estrategias y políticas de crecimiento y desarrollo económico y social que se determinen para el país.".</v>
       </c>
-      <c r="J300" s="1"/>
+      <c r="J300" s="1" t="s">
+        <v>453</v>
+      </c>
       <c r="K300" s="6">
         <v>9</v>
       </c>
@@ -22315,7 +22350,7 @@
         <v>No Contiene</v>
       </c>
     </row>
-    <row r="301" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:14" ht="24" x14ac:dyDescent="0.3">
       <c r="A301" s="2" t="s">
         <v>360</v>
       </c>
@@ -22341,7 +22376,9 @@
         <f>+LeyCC[[#This Row],[Artículo]]&amp;" ["&amp;LeyCC[[#This Row],[letra/número]]&amp;"] "&amp;LeyCC[[#This Row],[Texto Artículo]]</f>
         <v>Artículo 53 [2] En la letra g) del artículo 3°:</v>
       </c>
-      <c r="J301" s="1"/>
+      <c r="J301" s="1" t="s">
+        <v>453</v>
+      </c>
       <c r="K301" s="6">
         <v>9</v>
       </c>
@@ -22385,7 +22422,9 @@
         <v>Artículo 53 [2a] Reemplázase el párrafo primero por el siguiente:
 "g) Evaluar las iniciativas de inversión que soliciten financiamiento del Estado, para determinar su rentabilidad social y elaborar un informe al respecto, de conformidad con lo dispuesto en el artículo 19 bis del decreto ley N° 1.263, de 1975, Orgánico de Administración Financiera del Estado. En cumplimiento de lo anterior deberá establecer y actualizar los criterios y las metodologías aplicables en la referida evaluación. La determinación de estos criterios y metodologías deberá considerar especialmente la incorporación de indicadores objetivos y "comprobables respecto al desarrollo de las iniciativas de inversión, así como también el cumplimiento de los objetivos establecidos en la Estrategia Climática de Largo Plazo. Las metodologías y sus criterios de evaluación deberán mantenerse a disposición permanente del público en el sitio electrónico del Ministerio de Desarrollo Social y Familia.".</v>
       </c>
-      <c r="J302" s="1"/>
+      <c r="J302" s="1" t="s">
+        <v>453</v>
+      </c>
       <c r="K302" s="6">
         <v>9</v>
       </c>
@@ -22430,7 +22469,9 @@
 "En cumplimiento de lo anterior le corresponderá velar por que las iniciativas de inversión que utilicen financiamiento del Estado sean socialmente rentables y respondan a las políticas de crecimiento y desarrollo económico y social que se determinen para el país y sus regiones. Los Ministros de Desarrollo Social y Familia y de Hacienda, conjuntamente, establecerán directrices basadas en las características de las iniciativas de inversión a partir de las cuales no se les hará exigible el informe señalado en el párrafo anterior, las que serán revisadas anualmente y se mantendrán publicadas de conformidad al citado párrafo. Ambos ministerios realizarán esta revisión teniendo especial consideración de los objetivos, metas e indicadores establecidos por la Estrategia Climática de Largo Plazo y los Planes Sectoriales de Mitigación y Adaptación al Cambio Climático.
 Estas directrices se informarán a la Comisión Especial Mixta de Presupuestos, a más tardar, el 30 de noviembre de cada año.".</v>
       </c>
-      <c r="J303" s="1"/>
+      <c r="J303" s="1" t="s">
+        <v>453</v>
+      </c>
       <c r="K303" s="6">
         <v>9</v>
       </c>
@@ -22471,7 +22512,9 @@
         <v>Artículo 54. Agrégase, el siguiente literal s), nuevo, en el artículo 65 de la ley N° 18.695, orgánica constitucional de Municipalidades, sustituyéndose la expresión ", y" de la letra q) por un punto y coma, y el punto final de la letra r) por la siguiente expresión ", y":
 "s) Aprobar todos aquellos informes que le sean requeridos a la municipalidad en virtud de la Ley Marco Cambio Climático.".</v>
       </c>
-      <c r="J304" s="1"/>
+      <c r="J304" s="1" t="s">
+        <v>453</v>
+      </c>
       <c r="K304" s="6">
         <v>9</v>
       </c>
@@ -22508,7 +22551,9 @@
         <f>+LeyCC[[#This Row],[Artículo]]&amp;". "&amp;LeyCC[[#This Row],[Texto Artículo]]</f>
         <v>Artículo primero. La Estrategia Climática de Largo Plazo presentada ante la Convención Marco de Naciones Unidas sobre el Cambio Climático el 3 de noviembre del año 2021 mantendrá su vigencia para todos los efectos legales y deberá ser actualizada en el año 2030, de conformidad a esta ley. Por su parte, los Planes de Acción Regional sobre Cambio Climático que se encuentran en elaboración a la fecha de publicación de esta ley, se entenderá que cumplen con lo dispuesto en el artículo 11 y se actualizarán al año 2025.</v>
       </c>
-      <c r="J305" s="1"/>
+      <c r="J305" s="1" t="s">
+        <v>590</v>
+      </c>
       <c r="K305" s="6">
         <v>10</v>
       </c>
@@ -22543,7 +22588,9 @@
         <f>+LeyCC[[#This Row],[Artículo]]&amp;". "&amp;LeyCC[[#This Row],[Texto Artículo]]</f>
         <v>Artículo segundo. Los Planes Sectoriales de Mitigación y/o Adaptación deberán elaborarse en el plazo de dos años contado desde la publicación de la presente ley. Los Planes Sectoriales de Adaptación dictados con anterioridad a la entrada en vigencia de esta ley deberán ser actualizados en el mismo plazo establecido en el inciso anterior. Por su parte, los Planes de Acción Regional de Cambio Climático deberán elaborarse en el plazo de tres años contado desde la publicación de la Estrategia Climática de Largo Plazo.</v>
       </c>
-      <c r="J306" s="1"/>
+      <c r="J306" s="1" t="s">
+        <v>590</v>
+      </c>
       <c r="K306" s="6">
         <v>10</v>
       </c>
@@ -22578,7 +22625,9 @@
         <f>+LeyCC[[#This Row],[Artículo]]&amp;". "&amp;LeyCC[[#This Row],[Texto Artículo]]</f>
         <v>Artículo tercero. Los reglamentos establecidos en la presente ley se dictarán en el plazo de un año contado desde la publicación de la misma. Dichos reglamentos podrán ser agrupados en uno o más cuerpos reglamentarios, siempre que sean dictados por el mismo ministerio, regulando materias afines o relacionadas entre sí. Sin perjuicio de lo dispuesto en el inciso anterior, aquellos órganos y sistemas de información que estuvieren en funcionamiento al momento de la publicación de esta ley continuarán funcionando de acuerdo a sus reglas, hasta la dictación de los reglamentos correspondientes.</v>
       </c>
-      <c r="J307" s="1"/>
+      <c r="J307" s="1" t="s">
+        <v>590</v>
+      </c>
       <c r="K307" s="6">
         <v>10</v>
       </c>
@@ -22613,7 +22662,9 @@
         <f>+LeyCC[[#This Row],[Artículo]]&amp;". "&amp;LeyCC[[#This Row],[Texto Artículo]]</f>
         <v>Artículo cuarto. Las disposiciones de los artículos 40 y 46, N° 4, sólo entrarán en vigencia una vez que se dicte el reglamento a que hace referencia el artículo 40.</v>
       </c>
-      <c r="J308" s="1"/>
+      <c r="J308" s="1" t="s">
+        <v>590</v>
+      </c>
       <c r="K308" s="6">
         <v>10</v>
       </c>
@@ -22648,7 +22699,9 @@
         <f>+LeyCC[[#This Row],[Artículo]]&amp;". "&amp;LeyCC[[#This Row],[Texto Artículo]]</f>
         <v>Artículo quinto. El mayor gasto fiscal que represente la aplicación de la presente ley durante su primer año presupuestario de vigencia se financiará con cargo al presupuesto del Ministerio del Medio Ambiente. Con todo, el gasto relativo a planes y estrategias sectoriales se financiarán con cargo a las partidas presupuestarias de los Ministerios: de Energía, de Transportes y Telecomunicaciones, de Vivienda y Urbanismo, de Obras Públicas, de Salud, de Minería, de Agricultura, de Economía, Fomento y Turismo y de Defensa Nacional. En los años siguientes se financiará con cargo a los recursos que se establezcan en las respectivas leyes de presupuestos del sector público.</v>
       </c>
-      <c r="J309" s="1"/>
+      <c r="J309" s="1" t="s">
+        <v>590</v>
+      </c>
       <c r="K309" s="6">
         <v>10</v>
       </c>
@@ -22683,7 +22736,9 @@
         <f>+LeyCC[[#This Row],[Artículo]]&amp;". "&amp;LeyCC[[#This Row],[Texto Artículo]]</f>
         <v>Artículo sexto. El primer informe de inversión climática deberá elaborarse conforme a lo establecido en el artículo 38, y será presentado durante el primer mes de septiembre siguiente a la entrada en vigencia de la ley, o al subsiguiente si hubieran transcurrido menos de seis meses desde su entrada en vigencia."". Habiéndose cumplido con lo establecido en el Nº 1 del artículo 93 de la Constitución Política de la República y por cuanto he tenido a bien aprobarlo y sancionarlo; por tanto, promúlguese y llévese a efecto como Ley de la República.</v>
       </c>
-      <c r="J310" s="1"/>
+      <c r="J310" s="1" t="s">
+        <v>590</v>
+      </c>
       <c r="K310" s="6">
         <v>10</v>
       </c>

</xml_diff>